<commit_message>
updated docs, summaries, seperated apis
</commit_message>
<xml_diff>
--- a/interject.data.api/Examples/example.xlsx
+++ b/interject.data.api/Examples/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26818"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\samuelr\Documents\GitHub\ids-dotnet-api\Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\samuelr\Documents\GitHub\ids-dotnet-api\interject.data.api\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3879A017-F134-477E-9DCF-1225CE92EBAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5464E8FC-4E7F-4C14-8F54-74DE9F363016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27600" windowHeight="14205" activeTab="4" xr2:uid="{2C001AEE-9CFE-4283-8206-3A2DE5EB039F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27660" windowHeight="14205" activeTab="4" xr2:uid="{2C001AEE-9CFE-4283-8206-3A2DE5EB039F}"/>
   </bookViews>
   <sheets>
     <sheet name="ReportRange" sheetId="7" r:id="rId1"/>
@@ -285,7 +285,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="47">
   <si>
     <t>CompanyName:</t>
   </si>
@@ -341,9 +341,6 @@
     <t>Division</t>
   </si>
   <si>
-    <t>[!DetailRow]</t>
-  </si>
-  <si>
     <t>Save Results</t>
   </si>
   <si>
@@ -429,111 +426,6 @@
   </si>
   <si>
     <t>Company Name:</t>
-  </si>
-  <si>
-    <t>BOTTM</t>
-  </si>
-  <si>
-    <t>Bottom-Dollar Markets</t>
-  </si>
-  <si>
-    <t>Elizabeth Lincoln</t>
-  </si>
-  <si>
-    <t>Accounting Manager</t>
-  </si>
-  <si>
-    <t>23 Tsawassen Blvd.</t>
-  </si>
-  <si>
-    <t>Tsawassen</t>
-  </si>
-  <si>
-    <t>BC</t>
-  </si>
-  <si>
-    <t>T2F 8M4</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>(604) 555-4729</t>
-  </si>
-  <si>
-    <t>GREAL</t>
-  </si>
-  <si>
-    <t>Great Lakes Food Market</t>
-  </si>
-  <si>
-    <t>Howard Snyder</t>
-  </si>
-  <si>
-    <t>Marketing Manager</t>
-  </si>
-  <si>
-    <t>2732 Baker Blvd.</t>
-  </si>
-  <si>
-    <t>Eugene</t>
-  </si>
-  <si>
-    <t>OR</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>(503) 555-7555</t>
-  </si>
-  <si>
-    <t>SAVEA</t>
-  </si>
-  <si>
-    <t>Save-a-lot Markets</t>
-  </si>
-  <si>
-    <t>Jose Pavarotti</t>
-  </si>
-  <si>
-    <t>Sales Representative</t>
-  </si>
-  <si>
-    <t>187 Suffolk Ln.</t>
-  </si>
-  <si>
-    <t>Boise</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>(208) 555-8097</t>
-  </si>
-  <si>
-    <t>WHITC</t>
-  </si>
-  <si>
-    <t>White Clover Markets</t>
-  </si>
-  <si>
-    <t>Karl Jablonski</t>
-  </si>
-  <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>305 - 14th Ave. S. Suite 3B</t>
-  </si>
-  <si>
-    <t>Seattle</t>
-  </si>
-  <si>
-    <t>WA</t>
-  </si>
-  <si>
-    <t>(206) 555-4112</t>
   </si>
 </sst>
 </file>
@@ -672,9 +564,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -712,7 +604,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -818,7 +710,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -960,7 +852,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1170,7 +1062,7 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>1</v>
@@ -1401,10 +1293,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B6CE44-08AD-43F7-82DC-2D31087510A4}">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1420,7 +1312,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1440,15 +1332,15 @@
         <v>16</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1456,7 +1348,7 @@
         <v>12</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1466,12 +1358,12 @@
     </row>
     <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1484,16 +1376,16 @@
         <v>8</v>
       </c>
       <c r="D10" s="4" t="str">
-        <f ca="1">_xll.ReportVariable("DotNet_API_Variable",B23:B39,2:2,,_xll.Param(D17,D18,D19))</f>
+        <f ca="1">_xll.ReportVariable("DotNet_API_Variable",B23:B27,2:2,,_xll.Param(D17,D18,D19))</f>
         <v>OK!: ReportVariable Formula OK [jAction{}]</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C11" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="4" t="str">
-        <f ca="1">_xll.ReportSave("DotNet_API_Save",A23:A39,4:4,8:8,_xll.Param(D17,D18,D19))</f>
+        <f ca="1">_xll.ReportSave("DotNet_API_Save",A23:A27,4:4,8:8,_xll.Param(D17,D18,D19))</f>
         <v>OK!: ReportSave Formula OK [jAction{}]</v>
       </c>
     </row>
@@ -1555,10 +1447,10 @@
         <v>16</v>
       </c>
       <c r="G22" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="13" t="s">
         <v>25</v>
-      </c>
-      <c r="H22" s="13" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1569,324 +1461,36 @@
         <f>+A23</f>
         <v>701</v>
       </c>
-      <c r="C23">
-        <v>3333</v>
-      </c>
-      <c r="D23">
-        <v>94.34</v>
-      </c>
-      <c r="E23">
-        <v>904.34</v>
-      </c>
-      <c r="F23">
-        <v>9804.34</v>
-      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>701</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24">
-        <v>3334</v>
-      </c>
-      <c r="D24">
-        <v>94.34</v>
-      </c>
-      <c r="E24">
-        <v>904.34</v>
-      </c>
-      <c r="F24">
-        <v>9804.34</v>
+        <v>702</v>
+      </c>
+      <c r="B24" s="11">
+        <f>+A24</f>
+        <v>702</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>701</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25">
-        <v>3335</v>
-      </c>
-      <c r="D25">
-        <v>94.34</v>
-      </c>
-      <c r="E25">
-        <v>904.34</v>
-      </c>
-      <c r="F25">
-        <v>9804.34</v>
+        <v>703</v>
+      </c>
+      <c r="B25" s="11">
+        <f>+A25</f>
+        <v>703</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>701</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26">
-        <v>3336</v>
-      </c>
-      <c r="D26">
-        <v>94.34</v>
-      </c>
-      <c r="E26">
-        <v>904.34</v>
-      </c>
-      <c r="F26">
-        <v>9804.34</v>
+        <v>704</v>
+      </c>
+      <c r="B26" s="11">
+        <f>+A26</f>
+        <v>704</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>702</v>
-      </c>
-      <c r="B27" s="11">
-        <f>+A27</f>
-        <v>702</v>
-      </c>
-      <c r="C27">
-        <v>2333</v>
-      </c>
-      <c r="D27">
-        <v>94.34</v>
-      </c>
-      <c r="E27">
-        <v>904.34</v>
-      </c>
-      <c r="F27">
-        <v>9804.34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>702</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28">
-        <v>2334</v>
-      </c>
-      <c r="D28">
-        <v>94.34</v>
-      </c>
-      <c r="E28">
-        <v>904.34</v>
-      </c>
-      <c r="F28">
-        <v>9804.34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>702</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29">
-        <v>2335</v>
-      </c>
-      <c r="D29">
-        <v>94.34</v>
-      </c>
-      <c r="E29">
-        <v>904.34</v>
-      </c>
-      <c r="F29">
-        <v>9804.34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>702</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30">
-        <v>2336</v>
-      </c>
-      <c r="D30">
-        <v>94.34</v>
-      </c>
-      <c r="E30">
-        <v>904.34</v>
-      </c>
-      <c r="F30">
-        <v>9804.34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>703</v>
-      </c>
-      <c r="B31" s="11">
-        <f>+A31</f>
-        <v>703</v>
-      </c>
-      <c r="C31">
-        <v>1333</v>
-      </c>
-      <c r="D31">
-        <v>94.34</v>
-      </c>
-      <c r="E31">
-        <v>904.34</v>
-      </c>
-      <c r="F31">
-        <v>9804.34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>703</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32">
-        <v>1334</v>
-      </c>
-      <c r="D32">
-        <v>94.34</v>
-      </c>
-      <c r="E32">
-        <v>904.34</v>
-      </c>
-      <c r="F32">
-        <v>9804.34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>703</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33">
-        <v>1335</v>
-      </c>
-      <c r="D33">
-        <v>94.34</v>
-      </c>
-      <c r="E33">
-        <v>904.34</v>
-      </c>
-      <c r="F33">
-        <v>9804.34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>703</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34">
-        <v>1336</v>
-      </c>
-      <c r="D34">
-        <v>94.34</v>
-      </c>
-      <c r="E34">
-        <v>904.34</v>
-      </c>
-      <c r="F34">
-        <v>9804.34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>704</v>
-      </c>
-      <c r="B35" s="11">
-        <f>+A35</f>
-        <v>704</v>
-      </c>
-      <c r="C35">
-        <v>333</v>
-      </c>
-      <c r="D35">
-        <v>94.34</v>
-      </c>
-      <c r="E35">
-        <v>904.34</v>
-      </c>
-      <c r="F35">
-        <v>9804.34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>704</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C36">
-        <v>334</v>
-      </c>
-      <c r="D36">
-        <v>94.34</v>
-      </c>
-      <c r="E36">
-        <v>904.34</v>
-      </c>
-      <c r="F36">
-        <v>9804.34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>704</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37">
-        <v>335</v>
-      </c>
-      <c r="D37">
-        <v>94.34</v>
-      </c>
-      <c r="E37">
-        <v>904.34</v>
-      </c>
-      <c r="F37">
-        <v>9804.34</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>704</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38">
-        <v>336</v>
-      </c>
-      <c r="D38">
-        <v>94.34</v>
-      </c>
-      <c r="E38">
-        <v>904.34</v>
-      </c>
-      <c r="F38">
-        <v>9804.34</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="6"/>
+      <c r="B27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1896,10 +1500,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA7506E-D95C-4C04-BD41-F99F93279D9E}">
-  <dimension ref="B1:P22"/>
+  <dimension ref="B1:P19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1921,49 +1525,49 @@
     </row>
     <row r="2" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" spans="2:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1981,7 +1585,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="4" t="str">
-        <f ca="1">_xll.ReportRange("DotNet_API_SQL",18:22,2:2,,_xll.Param(D12,D13,D14))</f>
+        <f ca="1">_xll.ReportRange("DotNet_API_SQL",18:19,2:2,,_xll.Param(D12,D13,D14))</f>
         <v>OK!: ReportRange Formula OK [jAction{}]</v>
       </c>
     </row>
@@ -2022,241 +1626,53 @@
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="D17" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="E17" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="F17" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>46</v>
-      </c>
       <c r="J17" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="10" t="s">
+      <c r="L17" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="L17" s="10" t="s">
+      <c r="M17" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="M17" s="10" t="s">
+      <c r="N17" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="N17" s="10" t="s">
+      <c r="O17" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="O17" s="10" t="s">
+      <c r="P17" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="P17" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18" t="s">
-        <v>52</v>
-      </c>
-      <c r="G18" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" t="s">
-        <v>54</v>
-      </c>
-      <c r="I18" t="s">
-        <v>55</v>
-      </c>
-      <c r="J18" t="s">
-        <v>56</v>
-      </c>
-      <c r="K18" t="s">
-        <v>57</v>
-      </c>
-      <c r="L18">
-        <v>7174.74</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>8387.2000000000007</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" t="s">
-        <v>61</v>
-      </c>
-      <c r="F19" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" t="s">
-        <v>63</v>
-      </c>
-      <c r="H19" t="s">
-        <v>64</v>
-      </c>
-      <c r="I19">
-        <v>97403</v>
-      </c>
-      <c r="J19" t="s">
-        <v>65</v>
-      </c>
-      <c r="K19" t="s">
-        <v>66</v>
-      </c>
-      <c r="L19">
-        <v>15487.26</v>
-      </c>
-      <c r="M19">
-        <v>603.48</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" t="s">
-        <v>71</v>
-      </c>
-      <c r="G20" t="s">
-        <v>72</v>
-      </c>
-      <c r="H20" t="s">
-        <v>73</v>
-      </c>
-      <c r="I20">
-        <v>83720</v>
-      </c>
-      <c r="J20" t="s">
-        <v>65</v>
-      </c>
-      <c r="K20" t="s">
-        <v>74</v>
-      </c>
-      <c r="L20">
-        <v>42395.3</v>
-      </c>
-      <c r="M20">
-        <v>27574.52</v>
-      </c>
-      <c r="N20">
-        <v>7969.01</v>
-      </c>
-      <c r="O20">
-        <v>7329.17</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" t="s">
-        <v>78</v>
-      </c>
-      <c r="F21" t="s">
-        <v>79</v>
-      </c>
-      <c r="G21" t="s">
-        <v>80</v>
-      </c>
-      <c r="H21" t="s">
-        <v>81</v>
-      </c>
-      <c r="I21">
-        <v>98128</v>
-      </c>
-      <c r="J21" t="s">
-        <v>65</v>
-      </c>
-      <c r="K21" t="s">
-        <v>82</v>
-      </c>
-      <c r="L21">
-        <v>4552.2700000000004</v>
-      </c>
-      <c r="M21">
-        <v>3153.35</v>
-      </c>
-      <c r="N21">
-        <v>6795.58</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
+      <c r="B19" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed brackets and updated example.xlsx
</commit_message>
<xml_diff>
--- a/interject.data.api/Examples/example.xlsx
+++ b/interject.data.api/Examples/example.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26818"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27723"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\samuelr\Documents\GitHub\ids-dotnet-api\interject.data.api\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5464E8FC-4E7F-4C14-8F54-74DE9F363016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB455E5-1F09-41F1-928B-ABA3F9DAAFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27660" windowHeight="14205" activeTab="4" xr2:uid="{2C001AEE-9CFE-4283-8206-3A2DE5EB039F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27570" windowHeight="13530" xr2:uid="{2C001AEE-9CFE-4283-8206-3A2DE5EB039F}"/>
   </bookViews>
   <sheets>
     <sheet name="ReportRange" sheetId="7" r:id="rId1"/>
     <sheet name="ReportFixed" sheetId="3" r:id="rId2"/>
     <sheet name="ReportVariable" sheetId="4" r:id="rId3"/>
-    <sheet name="ReportSave" sheetId="5" r:id="rId4"/>
-    <sheet name="SQL" sheetId="6" r:id="rId5"/>
+    <sheet name="RowDef" sheetId="8" r:id="rId4"/>
+    <sheet name="RowDefName" sheetId="9" r:id="rId5"/>
+    <sheet name="ReportSave" sheetId="5" r:id="rId6"/>
+    <sheet name="SQL" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -192,6 +194,78 @@
     <author>Samuel Riesterer</author>
   </authors>
   <commentList>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{0103CBFC-B197-477C-A20A-997309C0AFA0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>search for company name. Use % for wildcard.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{AA25F0C8-D856-4C5D-9D35-5C8899D20A86}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>these are notes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Samuel Riesterer</author>
+  </authors>
+  <commentList>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{388A024E-477D-4ED4-84C0-FA42D5738244}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>search for company name. Use % for wildcard.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{51E1B4B1-A365-465A-A376-67767EA9A13A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>these are notes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Samuel Riesterer</author>
+  </authors>
+  <commentList>
     <comment ref="C10" authorId="0" shapeId="0" xr:uid="{62D6014E-8BD4-46D1-8796-2293D3145BA9}">
       <text>
         <r>
@@ -235,7 +309,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Samuel Riesterer</author>
@@ -284,8 +358,30 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="57">
   <si>
     <t>CompanyName:</t>
   </si>
@@ -426,6 +522,36 @@
   </si>
   <si>
     <t>Company Name:</t>
+  </si>
+  <si>
+    <t>loc</t>
+  </si>
+  <si>
+    <t>acct</t>
+  </si>
+  <si>
+    <t>Customer ID:</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>701|702</t>
+  </si>
+  <si>
+    <t>705|706|707</t>
+  </si>
+  <si>
+    <t>div</t>
+  </si>
+  <si>
+    <t>First rowdef</t>
+  </si>
+  <si>
+    <t>Second rowdef</t>
+  </si>
+  <si>
+    <t>Third rowdef</t>
   </si>
 </sst>
 </file>
@@ -862,9 +988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD67343-1597-4D18-9409-ED77D40D6A59}">
   <dimension ref="B1:F20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -995,9 +1119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DAF5BFD-5287-421E-826C-F1412B79DD79}">
   <dimension ref="B1:F22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1152,9 +1274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABAABD5A-0DED-4980-BC3C-B7E4F52D5CA2}">
   <dimension ref="B1:F22"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1292,12 +1412,385 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D0CD7E-3D61-41D3-B3B4-D9600C6BF780}">
+  <dimension ref="A1:I27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="C6" ca="1">_xll.ReportVariable("DotNet_API_rowdef",B17:B27,2:2,,_xll.Param(D11,D12,D13),,,TRUE)</f>
+        <v>OK!: ReportVariable Formula OK [jAction{}]</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="11"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="11"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="11">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="11"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="11">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="11"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="11"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="11">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{025A5458-442E-46FC-9A5F-03DBF67963BB}">
+  <dimension ref="A1:K23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="C6" ca="1">_xll.ReportVariable("DotNet_API_rowdefname",B17:C23,2:2,,_xll.Param(D11,D12,D13),,,TRUE)</f>
+        <v>OK!: ReportVariable Formula OK [jAction{}]</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="11"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="11"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="11"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B6CE44-08AD-43F7-82DC-2D31087510A4}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1498,13 +1991,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA7506E-D95C-4C04-BD41-F99F93279D9E}">
   <dimension ref="B1:P19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Added jDropdown and Parameters endpoint
</commit_message>
<xml_diff>
--- a/interject.data.api/Examples/example.xlsx
+++ b/interject.data.api/Examples/example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27723"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27809"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\samuelr\Documents\GitHub\ids-dotnet-api\interject.data.api\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB455E5-1F09-41F1-928B-ABA3F9DAAFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4609E979-33B4-41A7-8F20-674FDE5A3758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27570" windowHeight="13530" xr2:uid="{2C001AEE-9CFE-4283-8206-3A2DE5EB039F}"/>
   </bookViews>
@@ -16,11 +16,16 @@
     <sheet name="ReportRange" sheetId="7" r:id="rId1"/>
     <sheet name="ReportFixed" sheetId="3" r:id="rId2"/>
     <sheet name="ReportVariable" sheetId="4" r:id="rId3"/>
-    <sheet name="RowDef" sheetId="8" r:id="rId4"/>
-    <sheet name="RowDefName" sheetId="9" r:id="rId5"/>
-    <sheet name="ReportSave" sheetId="5" r:id="rId6"/>
-    <sheet name="SQL" sheetId="6" r:id="rId7"/>
+    <sheet name="ReportSave" sheetId="5" r:id="rId4"/>
+    <sheet name="jDropdown" sheetId="10" r:id="rId5"/>
+    <sheet name="Parameters" sheetId="11" r:id="rId6"/>
+    <sheet name="RowDef" sheetId="8" r:id="rId7"/>
+    <sheet name="RowDefName" sheetId="9" r:id="rId8"/>
+    <sheet name="SQL" sheetId="6" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="CompanyName" localSheetId="4">jDropdown!$D$6</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -194,78 +199,6 @@
     <author>Samuel Riesterer</author>
   </authors>
   <commentList>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{0103CBFC-B197-477C-A20A-997309C0AFA0}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>search for company name. Use % for wildcard.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{AA25F0C8-D856-4C5D-9D35-5C8899D20A86}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>these are notes</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Samuel Riesterer</author>
-  </authors>
-  <commentList>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{388A024E-477D-4ED4-84C0-FA42D5738244}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>search for company name. Use % for wildcard.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{51E1B4B1-A365-465A-A376-67767EA9A13A}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>these are notes</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Samuel Riesterer</author>
-  </authors>
-  <commentList>
     <comment ref="C10" authorId="0" shapeId="0" xr:uid="{62D6014E-8BD4-46D1-8796-2293D3145BA9}">
       <text>
         <r>
@@ -309,7 +242,138 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Samuel Riesterer</author>
+  </authors>
+  <commentList>
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{6EF12B30-6C70-4B4E-B0C2-CFCD1A9C19BD}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pull via API ReportFixed</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Samuel Riesterer</author>
+  </authors>
+  <commentList>
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{8D6632ED-4A26-4909-A9C8-4107BE51F11E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pull via API ReportFixed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{507BDBC1-1B5F-4875-BC58-6C701210BF3F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>search for company name. Use % for wildcard.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Samuel Riesterer</author>
+  </authors>
+  <commentList>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{0103CBFC-B197-477C-A20A-997309C0AFA0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>search for company name. Use % for wildcard.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{AA25F0C8-D856-4C5D-9D35-5C8899D20A86}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>these are notes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Samuel Riesterer</author>
+  </authors>
+  <commentList>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{388A024E-477D-4ED4-84C0-FA42D5738244}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>search for company name. Use % for wildcard.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{51E1B4B1-A365-465A-A376-67767EA9A13A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>these are notes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Samuel Riesterer</author>
@@ -381,7 +445,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="103">
   <si>
     <t>CompanyName:</t>
   </si>
@@ -552,13 +616,154 @@
   </si>
   <si>
     <t>Third rowdef</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>RowDefItems</t>
+  </si>
+  <si>
+    <t>ColDefItems</t>
+  </si>
+  <si>
+    <t>; Interject.Api.InterjectColDefItem; Interject.Api.InterjectColDefItem</t>
+  </si>
+  <si>
+    <t>ntLogin</t>
+  </si>
+  <si>
+    <t>samuelr</t>
+  </si>
+  <si>
+    <t>excelVersion</t>
+  </si>
+  <si>
+    <t>returnError</t>
+  </si>
+  <si>
+    <t>localTimeZoneOffset</t>
+  </si>
+  <si>
+    <t>sourceFileAndPath</t>
+  </si>
+  <si>
+    <t>D:\Users\samuelr\Documents\APIs|APITesting_v1.1.4.xlsx</t>
+  </si>
+  <si>
+    <t>sourceFilePathAndTab</t>
+  </si>
+  <si>
+    <t>D:\Users\samuelr\Documents\APIs|APITesting_v1.1.4.xlsx|.Net_Parameters</t>
+  </si>
+  <si>
+    <t>userID</t>
+  </si>
+  <si>
+    <t>U7v4kuw3IC</t>
+  </si>
+  <si>
+    <t>loginName</t>
+  </si>
+  <si>
+    <t>samuelr@gointerject.com</t>
+  </si>
+  <si>
+    <t>userRoles</t>
+  </si>
+  <si>
+    <t>ClientAdmin</t>
+  </si>
+  <si>
+    <t>clientID</t>
+  </si>
+  <si>
+    <t>CeAsHCdX</t>
+  </si>
+  <si>
+    <t>excelVersion2</t>
+  </si>
+  <si>
+    <t>userID2</t>
+  </si>
+  <si>
+    <t>clientID2</t>
+  </si>
+  <si>
+    <t>loginName2</t>
+  </si>
+  <si>
+    <t>machineLoginName</t>
+  </si>
+  <si>
+    <t>machineName</t>
+  </si>
+  <si>
+    <t>WSAMZN-UQTOQM95</t>
+  </si>
+  <si>
+    <t>fullName</t>
+  </si>
+  <si>
+    <t>Samuel Riesterer</t>
+  </si>
+  <si>
+    <t>loginDateUtc</t>
+  </si>
+  <si>
+    <t>userRoles2</t>
+  </si>
+  <si>
+    <t>idsVersion</t>
+  </si>
+  <si>
+    <t>2.5.1.1</t>
+  </si>
+  <si>
+    <t>fileName</t>
+  </si>
+  <si>
+    <t>APITesting_v1.1.4.xlsx</t>
+  </si>
+  <si>
+    <t>filePath</t>
+  </si>
+  <si>
+    <t>D:\Users\samuelr\Documents\APIs</t>
+  </si>
+  <si>
+    <t>tabName</t>
+  </si>
+  <si>
+    <t>.Net_Parameters</t>
+  </si>
+  <si>
+    <t>cellRange</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>sourceFunction</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>utcOffset</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -590,6 +795,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -648,10 +868,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -672,8 +894,20 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1412,12 +1646,632 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B6CE44-08AD-43F7-82DC-2D31087510A4}">
+  <dimension ref="B1:H27"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="34.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4" t="str">
+        <f ca="1">_xll.ReportVariable("DotNet_API_Variable",B23:B27,2:2,,_xll.Param(D17,D18,D19))</f>
+        <v>OK!: ReportVariable Formula OK [jAction{}]</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="4" t="str">
+        <f ca="1">_xll.ReportSave("DotNet_API_Save",A23:A27,4:4,8:8,_xll.Param(D17,D18,D19))</f>
+        <v>OK!: ReportSave Formula OK [jAction{}]</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="6"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="11">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="11">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="11">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="11">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8D515C2-F43A-428E-8B9B-F42EAD4B47A9}">
+  <dimension ref="B1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="D6" ca="1">_xll.jDropdown("DotNet_API_JDropdown",,,D12,"CompanyName")</f>
+        <v>&gt; jDropdown is ready for CompanyName at D12.</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="6"/>
+      <c r="C18" s="15"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C12" location="CompanyName" tooltip="Interject Dropdown" display="CompanyName:" xr:uid="{2E94A65A-4B3D-4183-B523-95A9CEF139EE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DBCAFA-2480-47EC-B897-A753DC42E540}">
+  <dimension ref="B1:E47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="72.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="str">
+        <f ca="1">_xll.ReportRange("DotNet_API_Parameters",18:46,2:2,,_xll.Param(D12,D13,D14))</f>
+        <v>OK!: ReportRange Formula OK [jAction{}]</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="16"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="16"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="16">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" s="16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="17">
+        <v>45447.38175925926</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45" s="16">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="8"/>
+      <c r="C46" s="16"/>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D0CD7E-3D61-41D3-B3B4-D9600C6BF780}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1598,7 +2452,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{025A5458-442E-46FC-9A5F-03DBF67963BB}">
   <dimension ref="A1:K23"/>
   <sheetViews>
@@ -1786,212 +2640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B6CE44-08AD-43F7-82DC-2D31087510A4}">
-  <dimension ref="A1:H27"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="34.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H8" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="4" t="str">
-        <f ca="1">_xll.ReportVariable("DotNet_API_Variable",B23:B27,2:2,,_xll.Param(D17,D18,D19))</f>
-        <v>OK!: ReportVariable Formula OK [jAction{}]</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="4" t="str">
-        <f ca="1">_xll.ReportSave("DotNet_API_Save",A23:A27,4:4,8:8,_xll.Param(D17,D18,D19))</f>
-        <v>OK!: ReportSave Formula OK [jAction{}]</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="H22" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>701</v>
-      </c>
-      <c r="B23" s="11">
-        <f>+A23</f>
-        <v>701</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>702</v>
-      </c>
-      <c r="B24" s="11">
-        <f>+A24</f>
-        <v>702</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>703</v>
-      </c>
-      <c r="B25" s="11">
-        <f>+A25</f>
-        <v>703</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>704</v>
-      </c>
-      <c r="B26" s="11">
-        <f>+A26</f>
-        <v>704</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA7506E-D95C-4C04-BD41-F99F93279D9E}">
   <dimension ref="B1:P19"/>
   <sheetViews>
@@ -1999,6 +2648,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>

</xml_diff>

<commit_message>
Added jdropdown and reportlookup to docs and examples
</commit_message>
<xml_diff>
--- a/interject.data.api/Examples/example.xlsx
+++ b/interject.data.api/Examples/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\samuelr\Documents\GitHub\ids-dotnet-api\interject.data.api\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4609E979-33B4-41A7-8F20-674FDE5A3758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFBC7E3-2202-495A-A3B1-3DDFE5E06333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27570" windowHeight="13530" xr2:uid="{2C001AEE-9CFE-4283-8206-3A2DE5EB039F}"/>
   </bookViews>
@@ -16,15 +16,17 @@
     <sheet name="ReportRange" sheetId="7" r:id="rId1"/>
     <sheet name="ReportFixed" sheetId="3" r:id="rId2"/>
     <sheet name="ReportVariable" sheetId="4" r:id="rId3"/>
-    <sheet name="ReportSave" sheetId="5" r:id="rId4"/>
-    <sheet name="jDropdown" sheetId="10" r:id="rId5"/>
-    <sheet name="Parameters" sheetId="11" r:id="rId6"/>
-    <sheet name="RowDef" sheetId="8" r:id="rId7"/>
-    <sheet name="RowDefName" sheetId="9" r:id="rId8"/>
-    <sheet name="SQL" sheetId="6" r:id="rId9"/>
+    <sheet name="ReportVariable (Multi-Cols)" sheetId="12" r:id="rId4"/>
+    <sheet name="ReportLookup" sheetId="13" r:id="rId5"/>
+    <sheet name="ReportSave" sheetId="5" r:id="rId6"/>
+    <sheet name="jDropdown" sheetId="10" r:id="rId7"/>
+    <sheet name="Parameters" sheetId="11" r:id="rId8"/>
+    <sheet name="RowDef" sheetId="8" r:id="rId9"/>
+    <sheet name="RowDefName" sheetId="9" r:id="rId10"/>
+    <sheet name="SQL" sheetId="6" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="CompanyName" localSheetId="4">jDropdown!$D$6</definedName>
+    <definedName name="CompanyName" localSheetId="6">jDropdown!$D$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -79,6 +81,91 @@
       </text>
     </comment>
     <comment ref="C13" authorId="0" shapeId="0" xr:uid="{CDDBC522-3818-4FEF-BD62-8106226747C9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>these are notes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Samuel Riesterer</author>
+  </authors>
+  <commentList>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{388A024E-477D-4ED4-84C0-FA42D5738244}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>search for company name. Use % for wildcard.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{51E1B4B1-A365-465A-A376-67767EA9A13A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>these are notes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Samuel Riesterer</author>
+  </authors>
+  <commentList>
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{A70DE517-D194-4562-9FEC-4017B9C0998A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pull via API ReportFixed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{D8A617D2-2911-457A-BAFC-9DD48A96BB1F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>search for company name. Use % for wildcard.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{70E1A113-2122-4FEB-B913-4D2A53BE9653}">
       <text>
         <r>
           <rPr>
@@ -199,6 +286,78 @@
     <author>Samuel Riesterer</author>
   </authors>
   <commentList>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{AAAF64DA-05C7-4014-9D60-14E158DE6321}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>search for company name. Use % for wildcard.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{1D83AEF0-09C9-49F5-8C2C-CF071A3363C3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>these are notes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Samuel Riesterer</author>
+  </authors>
+  <commentList>
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{5C876F75-6558-4149-B3E5-CF2264BD90C0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pull via API ReportFixed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{998A204B-1A6A-473D-9A6D-8DDFC7E0D0A5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>search for company name. Use % for wildcard.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Samuel Riesterer</author>
+  </authors>
+  <commentList>
     <comment ref="C10" authorId="0" shapeId="0" xr:uid="{62D6014E-8BD4-46D1-8796-2293D3145BA9}">
       <text>
         <r>
@@ -242,7 +401,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Samuel Riesterer</author>
@@ -265,7 +424,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Samuel Riesterer</author>
@@ -301,7 +460,7 @@
 </comments>
 </file>
 
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Samuel Riesterer</author>
@@ -321,91 +480,6 @@
       </text>
     </comment>
     <comment ref="C12" authorId="0" shapeId="0" xr:uid="{AA25F0C8-D856-4C5D-9D35-5C8899D20A86}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>these are notes</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Samuel Riesterer</author>
-  </authors>
-  <commentList>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{388A024E-477D-4ED4-84C0-FA42D5738244}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>search for company name. Use % for wildcard.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{51E1B4B1-A365-465A-A376-67767EA9A13A}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>these are notes</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Samuel Riesterer</author>
-  </authors>
-  <commentList>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{A70DE517-D194-4562-9FEC-4017B9C0998A}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Pull via API ReportFixed</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{D8A617D2-2911-457A-BAFC-9DD48A96BB1F}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>search for company name. Use % for wildcard.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{70E1A113-2122-4FEB-B913-4D2A53BE9653}">
       <text>
         <r>
           <rPr>
@@ -445,7 +519,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="104">
   <si>
     <t>CompanyName:</t>
   </si>
@@ -754,6 +828,9 @@
   </si>
   <si>
     <t>utcOffset</t>
+  </si>
+  <si>
+    <t>YTD:</t>
   </si>
 </sst>
 </file>
@@ -1226,6 +1303,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
@@ -1342,6 +1420,375 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{025A5458-442E-46FC-9A5F-03DBF67963BB}">
+  <dimension ref="A1:K23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="C6" ca="1">_xll.ReportVariable("DotNet_API_rowdefname",B17:C23,2:2,,_xll.Param(D11,D12,D13),,,TRUE)</f>
+        <v>OK!: ReportVariable Formula OK [jAction{}]</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="11"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="11"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="11"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA7506E-D95C-4C04-BD41-F99F93279D9E}">
+  <dimension ref="B1:P19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="str">
+        <f ca="1">_xll.ReportRange("DotNet_API_SQL",18:19,2:2,,_xll.Param(D12,D13,D14))</f>
+        <v>OK!: ReportRange Formula OK [jAction{}]</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="N17" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="O17" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="P17" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1357,6 +1804,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
@@ -1512,6 +1960,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
@@ -1646,6 +2095,321 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7E8EB36-3D35-47A5-8F38-75B6586307FF}">
+  <dimension ref="A1:I27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="C6" ca="1">_xll.ReportVariable("Dotnet_API_Variable",B17:C27,2:2,,_xll.Param(D11,D12,D13),,,TRUE)</f>
+        <v>OK!: ReportVariable Formula OK [jAction{}]</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="11">
+        <v>701</v>
+      </c>
+      <c r="C18" s="11">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="11">
+        <v>701</v>
+      </c>
+      <c r="C20" s="11">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="11">
+        <v>702</v>
+      </c>
+      <c r="C22" s="11">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="11">
+        <v>702</v>
+      </c>
+      <c r="C24" s="11">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="11">
+        <v>702</v>
+      </c>
+      <c r="C26" s="11">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B7BF0D-A97A-4DF3-8F5C-1F4E73F38D5E}">
+  <dimension ref="B1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="str">
+        <f ca="1">_xll.ReportLookup("DotNet_API_Lookup",C18,B2,_xll.Param(D12,D13,D14))</f>
+        <v>OK!: ReportLookup Formula OK [jAction{}]</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" s="15"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B6CE44-08AD-43F7-82DC-2D31087510A4}">
   <dimension ref="B1:H27"/>
   <sheetViews>
@@ -1653,7 +2417,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
@@ -1835,7 +2599,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8D515C2-F43A-428E-8B9B-F42EAD4B47A9}">
   <dimension ref="B1:E20"/>
   <sheetViews>
@@ -1843,7 +2607,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" customWidth="1"/>
@@ -1937,7 +2701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DBCAFA-2480-47EC-B897-A753DC42E540}">
   <dimension ref="B1:E47"/>
   <sheetViews>
@@ -1945,7 +2709,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="72.28515625" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
@@ -2267,7 +3031,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D0CD7E-3D61-41D3-B3B4-D9600C6BF780}">
   <dimension ref="A1:I27"/>
   <sheetViews>
@@ -2275,7 +3039,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.140625" customWidth="1"/>
@@ -2450,373 +3214,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{025A5458-442E-46FC-9A5F-03DBF67963BB}">
-  <dimension ref="A1:K23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="4" t="str" cm="1">
-        <f t="array" aca="1" ref="C6" ca="1">_xll.ReportVariable("DotNet_API_rowdefname",B17:C23,2:2,,_xll.Param(D11,D12,D13),,,TRUE)</f>
-        <v>OK!: ReportVariable Formula OK [jAction{}]</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K16" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="11"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="11"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="11"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA7506E-D95C-4C04-BD41-F99F93279D9E}">
-  <dimension ref="B1:P19"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="2:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="4" t="str">
-        <f ca="1">_xll.ReportRange("DotNet_API_SQL",18:19,2:2,,_xll.Param(D12,D13,D14))</f>
-        <v>OK!: ReportRange Formula OK [jAction{}]</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="K17" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="L17" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="M17" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N17" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="O17" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="P17" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
sync docs with other apis
</commit_message>
<xml_diff>
--- a/interject.data.api/Examples/example.xlsx
+++ b/interject.data.api/Examples/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\samuelr\Documents\GitHub\ids-dotnet-api\interject.data.api\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFBC7E3-2202-495A-A3B1-3DDFE5E06333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A958C47E-1C31-4C87-A980-1DDA78CE6F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27570" windowHeight="13530" xr2:uid="{2C001AEE-9CFE-4283-8206-3A2DE5EB039F}"/>
   </bookViews>
@@ -80,19 +80,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{CDDBC522-3818-4FEF-BD62-8106226747C9}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>these are notes</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -113,19 +100,6 @@
             <family val="2"/>
           </rPr>
           <t>search for company name. Use % for wildcard.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{51E1B4B1-A365-465A-A376-67767EA9A13A}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>these are notes</t>
         </r>
       </text>
     </comment>
@@ -165,19 +139,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{70E1A113-2122-4FEB-B913-4D2A53BE9653}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>these are notes</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -211,19 +172,6 @@
             <family val="2"/>
           </rPr>
           <t>search for company name. Use % for wildcard.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{086157AA-EB46-45DE-8C54-6050968727FB}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>these are notes</t>
         </r>
       </text>
     </comment>
@@ -263,19 +211,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{7754E789-DC93-4163-A1DE-8117CA4AAB17}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>these are notes</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -296,19 +231,6 @@
             <family val="2"/>
           </rPr>
           <t>search for company name. Use % for wildcard.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{1D83AEF0-09C9-49F5-8C2C-CF071A3363C3}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>these are notes</t>
         </r>
       </text>
     </comment>
@@ -381,19 +303,6 @@
             <family val="2"/>
           </rPr>
           <t>search for company name. Use % for wildcard.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C18" authorId="0" shapeId="0" xr:uid="{90E1CFF8-CF19-4B99-A50C-A9BFD33BD104}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>these are notes</t>
         </r>
       </text>
     </comment>
@@ -479,19 +388,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{AA25F0C8-D856-4C5D-9D35-5C8899D20A86}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>these are notes</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -519,7 +415,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="61">
   <si>
     <t>CompanyName:</t>
   </si>
@@ -698,139 +594,10 @@
     <t>Value</t>
   </si>
   <si>
-    <t>RowDefItems</t>
-  </si>
-  <si>
-    <t>ColDefItems</t>
-  </si>
-  <si>
-    <t>; Interject.Api.InterjectColDefItem; Interject.Api.InterjectColDefItem</t>
-  </si>
-  <si>
-    <t>ntLogin</t>
-  </si>
-  <si>
-    <t>samuelr</t>
-  </si>
-  <si>
-    <t>excelVersion</t>
-  </si>
-  <si>
-    <t>returnError</t>
-  </si>
-  <si>
-    <t>localTimeZoneOffset</t>
-  </si>
-  <si>
-    <t>sourceFileAndPath</t>
-  </si>
-  <si>
-    <t>D:\Users\samuelr\Documents\APIs|APITesting_v1.1.4.xlsx</t>
-  </si>
-  <si>
-    <t>sourceFilePathAndTab</t>
-  </si>
-  <si>
-    <t>D:\Users\samuelr\Documents\APIs|APITesting_v1.1.4.xlsx|.Net_Parameters</t>
-  </si>
-  <si>
-    <t>userID</t>
-  </si>
-  <si>
-    <t>U7v4kuw3IC</t>
-  </si>
-  <si>
-    <t>loginName</t>
-  </si>
-  <si>
-    <t>samuelr@gointerject.com</t>
-  </si>
-  <si>
-    <t>userRoles</t>
-  </si>
-  <si>
-    <t>ClientAdmin</t>
-  </si>
-  <si>
-    <t>clientID</t>
-  </si>
-  <si>
-    <t>CeAsHCdX</t>
-  </si>
-  <si>
-    <t>excelVersion2</t>
-  </si>
-  <si>
-    <t>userID2</t>
-  </si>
-  <si>
-    <t>clientID2</t>
-  </si>
-  <si>
-    <t>loginName2</t>
-  </si>
-  <si>
-    <t>machineLoginName</t>
-  </si>
-  <si>
-    <t>machineName</t>
-  </si>
-  <si>
-    <t>WSAMZN-UQTOQM95</t>
-  </si>
-  <si>
-    <t>fullName</t>
-  </si>
-  <si>
-    <t>Samuel Riesterer</t>
-  </si>
-  <si>
-    <t>loginDateUtc</t>
-  </si>
-  <si>
-    <t>userRoles2</t>
-  </si>
-  <si>
-    <t>idsVersion</t>
-  </si>
-  <si>
-    <t>2.5.1.1</t>
-  </si>
-  <si>
-    <t>fileName</t>
-  </si>
-  <si>
-    <t>APITesting_v1.1.4.xlsx</t>
-  </si>
-  <si>
-    <t>filePath</t>
-  </si>
-  <si>
-    <t>D:\Users\samuelr\Documents\APIs</t>
-  </si>
-  <si>
-    <t>tabName</t>
-  </si>
-  <si>
-    <t>.Net_Parameters</t>
-  </si>
-  <si>
-    <t>cellRange</t>
-  </si>
-  <si>
-    <t>D7</t>
-  </si>
-  <si>
-    <t>sourceFunction</t>
-  </si>
-  <si>
-    <t>Range</t>
-  </si>
-  <si>
-    <t>utcOffset</t>
-  </si>
-  <si>
     <t>YTD:</t>
+  </si>
+  <si>
+    <t>Parameter</t>
   </si>
 </sst>
 </file>
@@ -950,7 +717,7 @@
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -976,9 +743,6 @@
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1299,7 +1063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD67343-1597-4D18-9409-ED77D40D6A59}">
   <dimension ref="B1:F20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1318,10 +1082,10 @@
     </row>
     <row r="2" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>14</v>
@@ -1492,7 +1256,7 @@
     </row>
     <row r="6" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="str" cm="1">
-        <f t="array" aca="1" ref="C6" ca="1">_xll.ReportVariable("DotNet_API_rowdefname",B17:C23,2:2,,_xll.Param(D11,D12,D13),,,TRUE)</f>
+        <f t="array" aca="1" ref="C6" ca="1">_xll.ReportVariable("DotNet_API_RowDefName",B17:C23,2:2,,_xll.Param(D11,D12,D13),,,TRUE)</f>
         <v>OK!: ReportVariable Formula OK [jAction{}]</v>
       </c>
     </row>
@@ -1619,7 +1383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA7506E-D95C-4C04-BD41-F99F93279D9E}">
   <dimension ref="B1:P19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1720,7 +1484,9 @@
       <c r="C12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
@@ -1800,7 +1566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DAF5BFD-5287-421E-826C-F1412B79DD79}">
   <dimension ref="B1:F22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1819,10 +1585,10 @@
     </row>
     <row r="2" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>14</v>
@@ -1956,7 +1722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABAABD5A-0DED-4980-BC3C-B7E4F52D5CA2}">
   <dimension ref="B1:F22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1975,10 +1741,10 @@
     </row>
     <row r="2" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>14</v>
@@ -2393,7 +2159,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
-        <v>103</v>
+        <v>59</v>
       </c>
       <c r="C18" s="15"/>
     </row>
@@ -2413,7 +2179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B6CE44-08AD-43F7-82DC-2D31087510A4}">
   <dimension ref="B1:H27"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2703,7 +2469,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DBCAFA-2480-47EC-B897-A753DC42E540}">
-  <dimension ref="B1:E47"/>
+  <dimension ref="B1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2724,7 +2490,7 @@
     </row>
     <row r="2" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>58</v>
@@ -2745,7 +2511,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="4" t="str">
-        <f ca="1">_xll.ReportRange("DotNet_API_Parameters",18:46,2:2,,_xll.Param(D12,D13,D14))</f>
+        <f ca="1">_xll.ReportRange("DotNet_API_Parameters",18:19,2:2,,_xll.Param(D12,D13,D14))</f>
         <v>OK!: ReportRange Formula OK [jAction{}]</v>
       </c>
     </row>
@@ -2799,231 +2565,15 @@
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
-        <v>59</v>
-      </c>
+      <c r="B18" s="8"/>
       <c r="C18" s="16"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>61</v>
-      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="16"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" s="16">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="16"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="16">
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C30" s="16">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37" s="17">
-        <v>45447.38175925926</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C44" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C45" s="16">
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="8"/>
-      <c r="C46" s="16"/>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="6"/>
+      <c r="B20" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3086,7 +2636,7 @@
     </row>
     <row r="6" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="str" cm="1">
-        <f t="array" aca="1" ref="C6" ca="1">_xll.ReportVariable("DotNet_API_rowdef",B17:B27,2:2,,_xll.Param(D11,D12,D13),,,TRUE)</f>
+        <f t="array" aca="1" ref="C6" ca="1">_xll.ReportVariable("DotNet_API_RowDef",B17:B27,2:2,,_xll.Param(D11,D12,D13),,,TRUE)</f>
         <v>OK!: ReportVariable Formula OK [jAction{}]</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ijp 3507 update (#27)
* Added jDropdown and Parameters endpoint

* Added jdropdown and reportlookup to docs and examples

* sync docs with other apis
</commit_message>
<xml_diff>
--- a/interject.data.api/Examples/example.xlsx
+++ b/interject.data.api/Examples/example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27723"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27809"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\samuelr\Documents\GitHub\ids-dotnet-api\interject.data.api\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB455E5-1F09-41F1-928B-ABA3F9DAAFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A958C47E-1C31-4C87-A980-1DDA78CE6F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27570" windowHeight="13530" xr2:uid="{2C001AEE-9CFE-4283-8206-3A2DE5EB039F}"/>
   </bookViews>
@@ -16,11 +16,18 @@
     <sheet name="ReportRange" sheetId="7" r:id="rId1"/>
     <sheet name="ReportFixed" sheetId="3" r:id="rId2"/>
     <sheet name="ReportVariable" sheetId="4" r:id="rId3"/>
-    <sheet name="RowDef" sheetId="8" r:id="rId4"/>
-    <sheet name="RowDefName" sheetId="9" r:id="rId5"/>
+    <sheet name="ReportVariable (Multi-Cols)" sheetId="12" r:id="rId4"/>
+    <sheet name="ReportLookup" sheetId="13" r:id="rId5"/>
     <sheet name="ReportSave" sheetId="5" r:id="rId6"/>
-    <sheet name="SQL" sheetId="6" r:id="rId7"/>
+    <sheet name="jDropdown" sheetId="10" r:id="rId7"/>
+    <sheet name="Parameters" sheetId="11" r:id="rId8"/>
+    <sheet name="RowDef" sheetId="8" r:id="rId9"/>
+    <sheet name="RowDefName" sheetId="9" r:id="rId10"/>
+    <sheet name="SQL" sheetId="6" r:id="rId11"/>
   </sheets>
+  <definedNames>
+    <definedName name="CompanyName" localSheetId="6">jDropdown!$D$6</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -73,7 +80,17 @@
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{CDDBC522-3818-4FEF-BD62-8106226747C9}">
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Samuel Riesterer</author>
+  </authors>
+  <commentList>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{388A024E-477D-4ED4-84C0-FA42D5738244}">
       <text>
         <r>
           <rPr>
@@ -82,7 +99,43 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>these are notes</t>
+          <t>search for company name. Use % for wildcard.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Samuel Riesterer</author>
+  </authors>
+  <commentList>
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{A70DE517-D194-4562-9FEC-4017B9C0998A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pull via API ReportFixed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{D8A617D2-2911-457A-BAFC-9DD48A96BB1F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>search for company name. Use % for wildcard.</t>
         </r>
       </text>
     </comment>
@@ -122,19 +175,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{086157AA-EB46-45DE-8C54-6050968727FB}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>these are notes</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -171,19 +211,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{7754E789-DC93-4163-A1DE-8117CA4AAB17}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>these are notes</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -194,7 +221,7 @@
     <author>Samuel Riesterer</author>
   </authors>
   <commentList>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{0103CBFC-B197-477C-A20A-997309C0AFA0}">
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{AAAF64DA-05C7-4014-9D60-14E158DE6321}">
       <text>
         <r>
           <rPr>
@@ -204,19 +231,6 @@
             <family val="2"/>
           </rPr>
           <t>search for company name. Use % for wildcard.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{AA25F0C8-D856-4C5D-9D35-5C8899D20A86}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>these are notes</t>
         </r>
       </text>
     </comment>
@@ -230,7 +244,20 @@
     <author>Samuel Riesterer</author>
   </authors>
   <commentList>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{388A024E-477D-4ED4-84C0-FA42D5738244}">
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{5C876F75-6558-4149-B3E5-CF2264BD90C0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pull via API ReportFixed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{998A204B-1A6A-473D-9A6D-8DDFC7E0D0A5}">
       <text>
         <r>
           <rPr>
@@ -240,19 +267,6 @@
             <family val="2"/>
           </rPr>
           <t>search for company name. Use % for wildcard.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{51E1B4B1-A365-465A-A376-67767EA9A13A}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>these are notes</t>
         </r>
       </text>
     </comment>
@@ -292,19 +306,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="C18" authorId="0" shapeId="0" xr:uid="{90E1CFF8-CF19-4B99-A50C-A9BFD33BD104}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>these are notes</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -315,7 +316,7 @@
     <author>Samuel Riesterer</author>
   </authors>
   <commentList>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{A70DE517-D194-4562-9FEC-4017B9C0998A}">
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{6EF12B30-6C70-4B4E-B0C2-CFCD1A9C19BD}">
       <text>
         <r>
           <rPr>
@@ -328,7 +329,30 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{D8A617D2-2911-457A-BAFC-9DD48A96BB1F}">
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Samuel Riesterer</author>
+  </authors>
+  <commentList>
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{8D6632ED-4A26-4909-A9C8-4107BE51F11E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pull via API ReportFixed</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{507BDBC1-1B5F-4875-BC58-6C701210BF3F}">
       <text>
         <r>
           <rPr>
@@ -341,7 +365,17 @@
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{70E1A113-2122-4FEB-B913-4D2A53BE9653}">
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Samuel Riesterer</author>
+  </authors>
+  <commentList>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{0103CBFC-B197-477C-A20A-997309C0AFA0}">
       <text>
         <r>
           <rPr>
@@ -350,7 +384,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>these are notes</t>
+          <t>search for company name. Use % for wildcard.</t>
         </r>
       </text>
     </comment>
@@ -381,7 +415,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="61">
   <si>
     <t>CompanyName:</t>
   </si>
@@ -552,13 +586,28 @@
   </si>
   <si>
     <t>Third rowdef</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>YTD:</t>
+  </si>
+  <si>
+    <t>Parameter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -590,6 +639,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -648,10 +712,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -672,8 +738,17 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -988,10 +1063,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD67343-1597-4D18-9409-ED77D40D6A59}">
   <dimension ref="B1:F20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
@@ -1006,10 +1082,10 @@
     </row>
     <row r="2" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>14</v>
@@ -1115,490 +1191,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DAF5BFD-5287-421E-826C-F1412B79DD79}">
-  <dimension ref="B1:F22"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="4" t="str">
-        <f ca="1">_xll.ReportFixed("DotNet_API_Fixed",B18:C21,2:2,_xll.Param(D12,D13,D14))</f>
-        <v>OK!: ReportFixed Formula OK [jAction{}]</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="8">
-        <v>701</v>
-      </c>
-      <c r="C18" s="9">
-        <v>3339</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="8">
-        <v>701</v>
-      </c>
-      <c r="C19" s="9">
-        <v>3340</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="8">
-        <v>702</v>
-      </c>
-      <c r="C20" s="9">
-        <v>3339</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="8">
-        <v>702</v>
-      </c>
-      <c r="C21" s="9">
-        <v>3340</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABAABD5A-0DED-4980-BC3C-B7E4F52D5CA2}">
-  <dimension ref="B1:F22"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="4" t="str">
-        <f ca="1">_xll.ReportVariable("DotNet_API_Variable",B18:B22,2:2,,_xll.Param(D12,D13,D14))</f>
-        <v>OK!: ReportVariable Formula OK [jAction{}]</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="11">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="11">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="11">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="11">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D0CD7E-3D61-41D3-B3B4-D9600C6BF780}">
-  <dimension ref="A1:I27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="4" t="str" cm="1">
-        <f t="array" aca="1" ref="C6" ca="1">_xll.ReportVariable("DotNet_API_rowdef",B17:B27,2:2,,_xll.Param(D11,D12,D13),,,TRUE)</f>
-        <v>OK!: ReportVariable Formula OK [jAction{}]</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="11"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="11"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="11">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="11"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="11">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="11"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="11"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="11">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="11"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{025A5458-442E-46FC-9A5F-03DBF67963BB}">
   <dimension ref="A1:K23"/>
   <sheetViews>
@@ -1606,7 +1199,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.140625" customWidth="1"/>
@@ -1663,7 +1256,7 @@
     </row>
     <row r="6" spans="2:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="str" cm="1">
-        <f t="array" aca="1" ref="C6" ca="1">_xll.ReportVariable("DotNet_API_rowdefname",B17:C23,2:2,,_xll.Param(D11,D12,D13),,,TRUE)</f>
+        <f t="array" aca="1" ref="C6" ca="1">_xll.ReportVariable("DotNet_API_RowDefName",B17:C23,2:2,,_xll.Param(D11,D12,D13),,,TRUE)</f>
         <v>OK!: ReportVariable Formula OK [jAction{}]</v>
       </c>
     </row>
@@ -1786,219 +1379,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B6CE44-08AD-43F7-82DC-2D31087510A4}">
-  <dimension ref="A1:H27"/>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA7506E-D95C-4C04-BD41-F99F93279D9E}">
+  <dimension ref="B1:P19"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="34.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H8" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="4" t="str">
-        <f ca="1">_xll.ReportVariable("DotNet_API_Variable",B23:B27,2:2,,_xll.Param(D17,D18,D19))</f>
-        <v>OK!: ReportVariable Formula OK [jAction{}]</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="4" t="str">
-        <f ca="1">_xll.ReportSave("DotNet_API_Save",A23:A27,4:4,8:8,_xll.Param(D17,D18,D19))</f>
-        <v>OK!: ReportSave Formula OK [jAction{}]</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="H22" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>701</v>
-      </c>
-      <c r="B23" s="11">
-        <f>+A23</f>
-        <v>701</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>702</v>
-      </c>
-      <c r="B24" s="11">
-        <f>+A24</f>
-        <v>702</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>703</v>
-      </c>
-      <c r="B25" s="11">
-        <f>+A25</f>
-        <v>703</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>704</v>
-      </c>
-      <c r="B26" s="11">
-        <f>+A26</f>
-        <v>704</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA7506E-D95C-4C04-BD41-F99F93279D9E}">
-  <dimension ref="B1:P19"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
@@ -2095,7 +1484,9 @@
       <c r="C12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
@@ -2164,6 +1555,1210 @@
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DAF5BFD-5287-421E-826C-F1412B79DD79}">
+  <dimension ref="B1:F22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="str">
+        <f ca="1">_xll.ReportFixed("DotNet_API_Fixed",B18:C21,2:2,_xll.Param(D12,D13,D14))</f>
+        <v>OK!: ReportFixed Formula OK [jAction{}]</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="8">
+        <v>701</v>
+      </c>
+      <c r="C18" s="9">
+        <v>3339</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="8">
+        <v>701</v>
+      </c>
+      <c r="C19" s="9">
+        <v>3340</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="8">
+        <v>702</v>
+      </c>
+      <c r="C20" s="9">
+        <v>3339</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="8">
+        <v>702</v>
+      </c>
+      <c r="C21" s="9">
+        <v>3340</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABAABD5A-0DED-4980-BC3C-B7E4F52D5CA2}">
+  <dimension ref="B1:F22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="str">
+        <f ca="1">_xll.ReportVariable("DotNet_API_Variable",B18:B22,2:2,,_xll.Param(D12,D13,D14))</f>
+        <v>OK!: ReportVariable Formula OK [jAction{}]</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="11">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="11">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="11">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="11">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7E8EB36-3D35-47A5-8F38-75B6586307FF}">
+  <dimension ref="A1:I27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="C6" ca="1">_xll.ReportVariable("Dotnet_API_Variable",B17:C27,2:2,,_xll.Param(D11,D12,D13),,,TRUE)</f>
+        <v>OK!: ReportVariable Formula OK [jAction{}]</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="11">
+        <v>701</v>
+      </c>
+      <c r="C18" s="11">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="11">
+        <v>701</v>
+      </c>
+      <c r="C20" s="11">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="11">
+        <v>702</v>
+      </c>
+      <c r="C22" s="11">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="11">
+        <v>702</v>
+      </c>
+      <c r="C24" s="11">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="11">
+        <v>702</v>
+      </c>
+      <c r="C26" s="11">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B7BF0D-A97A-4DF3-8F5C-1F4E73F38D5E}">
+  <dimension ref="B1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="str">
+        <f ca="1">_xll.ReportLookup("DotNet_API_Lookup",C18,B2,_xll.Param(D12,D13,D14))</f>
+        <v>OK!: ReportLookup Formula OK [jAction{}]</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="15"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B6CE44-08AD-43F7-82DC-2D31087510A4}">
+  <dimension ref="B1:H27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="34.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4" t="str">
+        <f ca="1">_xll.ReportVariable("DotNet_API_Variable",B23:B27,2:2,,_xll.Param(D17,D18,D19))</f>
+        <v>OK!: ReportVariable Formula OK [jAction{}]</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="4" t="str">
+        <f ca="1">_xll.ReportSave("DotNet_API_Save",A23:A27,4:4,8:8,_xll.Param(D17,D18,D19))</f>
+        <v>OK!: ReportSave Formula OK [jAction{}]</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="6"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="11">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="11">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="11">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="11">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8D515C2-F43A-428E-8B9B-F42EAD4B47A9}">
+  <dimension ref="B1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="D6" ca="1">_xll.jDropdown("DotNet_API_JDropdown",,,D12,"CompanyName")</f>
+        <v>&gt; jDropdown is ready for CompanyName at D12.</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="6"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="6"/>
+      <c r="C18" s="15"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C12" location="CompanyName" tooltip="Interject Dropdown" display="CompanyName:" xr:uid="{2E94A65A-4B3D-4183-B523-95A9CEF139EE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DBCAFA-2480-47EC-B897-A753DC42E540}">
+  <dimension ref="B1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="72.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="str">
+        <f ca="1">_xll.ReportRange("DotNet_API_Parameters",18:19,2:2,,_xll.Param(D12,D13,D14))</f>
+        <v>OK!: ReportRange Formula OK [jAction{}]</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
+      <c r="C18" s="16"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+      <c r="C19" s="16"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D0CD7E-3D61-41D3-B3B4-D9600C6BF780}">
+  <dimension ref="A1:I27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="C6" ca="1">_xll.ReportVariable("DotNet_API_RowDef",B17:B27,2:2,,_xll.Param(D11,D12,D13),,,TRUE)</f>
+        <v>OK!: ReportVariable Formula OK [jAction{}]</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="11"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="11"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="11">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="11"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="11">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="11"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="11"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="11">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>